<commit_message>
JinL - fix some data import issues.
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/calphi/classLevel.xlsx
+++ b/data-transfer/transfer/data/calphi/classLevel.xlsx
@@ -471,7 +471,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G2" s="3">
         <v>4</v>

</xml_diff>